<commit_message>
updated mdl, bgdpbes, mppc, syshecf, tts, bdesc, cdrdfrcp, brzspbs
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\CO\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66CC60D9-AB82-4C6D-8771-9CBFFE207C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13631A39-D54F-4C89-8E6E-F4A9B84BEFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13395" yWindow="345" windowWidth="15360" windowHeight="16755" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="12330" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
         <v>60</v>
       </c>
       <c r="C1" s="7">
-        <v>45236</v>
+        <v>45265</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
   <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:AK22"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="J3:AK10" si="1">$B3</f>
+        <f t="shared" ref="J3:AK9" si="1">$B3</f>
         <v>0</v>
       </c>
       <c r="T3">
@@ -3719,140 +3719,112 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
-        <f t="shared" ref="G10:AK15" si="2">$B10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -3860,138 +3832,112 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -4003,143 +3949,143 @@
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:I12" si="3">$B12</f>
+        <f t="shared" ref="C12:I12" si="2">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G12:AK15" si="3">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="V12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="W12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="X12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
     </row>
@@ -4163,127 +4109,127 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4316,115 +4262,115 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4460,111 +4406,111 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>